<commit_message>
uploading test case stuff
</commit_message>
<xml_diff>
--- a/Documentation/Design Documents/TestCaseTemp.xlsx
+++ b/Documentation/Design Documents/TestCaseTemp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\School\Fall 2014\Sr. Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\CapStone\Documentation\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Project Name:</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Test Excution Date:</t>
+  </si>
+  <si>
+    <t>Requirement Satisfied:</t>
   </si>
 </sst>
 </file>
@@ -261,15 +264,25 @@
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -279,16 +292,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,18 +589,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -612,79 +615,79 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="2" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="8" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -714,171 +717,193 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="A21" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A12:G12"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E3:G3"/>
@@ -886,13 +911,6 @@
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>